<commit_message>
Seguimiento - Guion 9
Fechas de entrega de los documentos correspondientes al guion 9 del
grado 11
</commit_message>
<xml_diff>
--- a/seguimiento/Grado11.xlsx
+++ b/seguimiento/Grado11.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\seguimiento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\seguimiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10826" windowHeight="2872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="2865"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Editorial</t>
   </si>
@@ -64,6 +63,12 @@
   </si>
   <si>
     <t>Grado:</t>
+  </si>
+  <si>
+    <t>Ciencias Naturales</t>
+  </si>
+  <si>
+    <t>Se realizo modificación a la solicitud gráfica (cuaderno de estudio) 13/03/15</t>
   </si>
 </sst>
 </file>
@@ -441,62 +446,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,48 +552,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,357 +837,371 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="11.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.19921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.73046875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="36" t="s">
+      <c r="C1" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="37" t="s">
+      <c r="C2" s="34">
+        <v>11</v>
+      </c>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26" t="s">
+      <c r="J4" s="39"/>
+      <c r="K4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="26"/>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="37"/>
-      <c r="B5" s="27" t="s">
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36"/>
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="38">
+    <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="38">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="38">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="38">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
         <v>4</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="38">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
         <v>5</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="38">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="38">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="38">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="38">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29">
         <v>9</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="38">
+      <c r="B14" s="4">
+        <v>42076</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42076</v>
+      </c>
+      <c r="D14" s="5">
+        <v>42076</v>
+      </c>
+      <c r="E14" s="5">
+        <v>42075</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
         <v>10</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="38">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29">
         <v>11</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="38">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29">
         <v>12</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="38">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
         <v>13</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="38">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29">
         <v>14</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="38">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29">
         <v>15</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="39">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30">
         <v>16</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="18"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1201,7 +1220,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:E21 G6:G21 K6:K21">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K21 G6:G21 B6:E21">
       <formula1>42005</formula1>
       <formula2>42461</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Relación solicitud gráfica CN_11_12
Relación solicitud gráfica CN_11_12
</commit_message>
<xml_diff>
--- a/seguimiento/Grado11.xlsx
+++ b/seguimiento/Grado11.xlsx
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H17" sqref="H16:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1154,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5">
+        <v>42179</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="10"/>
       <c r="H17" s="11"/>

</xml_diff>